<commit_message>
Added new MA Cross over indicator amongst other changes
</commit_message>
<xml_diff>
--- a/cAlgo.Library/Robots/Analysis Queries/Database Analysis.xlsx
+++ b/cAlgo.Library/Robots/Analysis Queries/Database Analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rob\Documents\cAlgo\Sources\Robots\WaveCatcher\WaveCatcher\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rob\Documents\Visual Studio 2017\Projects\MetaTraderStrategies\cAlgo.Library\Robots\Analysis Queries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{30D0A378-2795-4800-ACAF-E1016C0FEE88}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D7D643-6ACD-4C0F-9651-60ED6D5EE5C6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="5" xr2:uid="{B8BC681A-5E76-45D5-BBB5-3F9FB8AF6CF2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{B8BC681A-5E76-45D5-BBB5-3F9FB8AF6CF2}"/>
   </bookViews>
   <sheets>
     <sheet name="H4 Analysis 1" sheetId="3" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Top Trades" sheetId="4" r:id="rId4"/>
     <sheet name="Range Analysis" sheetId="5" r:id="rId5"/>
     <sheet name="Close off High Analysis" sheetId="6" r:id="rId6"/>
+    <sheet name="H4RSI Analysis" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="52">
   <si>
     <t>RSIBand</t>
   </si>
@@ -598,7 +599,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'RSI Analysis'!$C$1</c15:sqref>
@@ -625,7 +626,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'RSI Analysis'!$A$2:$A$7</c15:sqref>
@@ -657,7 +658,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'RSI Analysis'!$C$2:$C$7</c15:sqref>
@@ -688,7 +689,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-C609-4BC5-B89B-975372AD8332}"/>
                   </c:ext>
@@ -701,7 +702,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'RSI Analysis'!$F$1</c15:sqref>
@@ -730,7 +731,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'RSI Analysis'!$A$2:$A$7</c15:sqref>
@@ -762,7 +763,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'RSI Analysis'!$F$2:$F$7</c15:sqref>
@@ -793,7 +794,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-C609-4BC5-B89B-975372AD8332}"/>
                   </c:ext>
@@ -1875,7 +1876,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D45D02F5-FD40-4467-9127-03C9DDEAD333}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -2193,7 +2194,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3845,7 +3846,7 @@
         <v>252632</v>
       </c>
       <c r="E2" s="1">
-        <f>C2/B2</f>
+        <f t="shared" ref="E2:E8" si="0">C2/B2</f>
         <v>0.28311823929353808</v>
       </c>
     </row>
@@ -3863,7 +3864,7 @@
         <v>343807</v>
       </c>
       <c r="E3" s="1">
-        <f>C3/B3</f>
+        <f t="shared" si="0"/>
         <v>0.29374365758563031</v>
       </c>
     </row>
@@ -3881,7 +3882,7 @@
         <v>90064</v>
       </c>
       <c r="E4" s="1">
-        <f>C4/B4</f>
+        <f t="shared" si="0"/>
         <v>0.35545186499871184</v>
       </c>
     </row>
@@ -3899,7 +3900,7 @@
         <v>27083</v>
       </c>
       <c r="E5" s="1">
-        <f>C5/B5</f>
+        <f t="shared" si="0"/>
         <v>0.38505029404418611</v>
       </c>
     </row>
@@ -3917,7 +3918,7 @@
         <v>9087</v>
       </c>
       <c r="E6" s="1">
-        <f>C6/B6</f>
+        <f t="shared" si="0"/>
         <v>0.49243143607216666</v>
       </c>
     </row>
@@ -3935,7 +3936,7 @@
         <v>183</v>
       </c>
       <c r="E7" s="1">
-        <f>C7/B7</f>
+        <f t="shared" si="0"/>
         <v>0.54590570719602982</v>
       </c>
     </row>
@@ -3953,7 +3954,7 @@
         <v>219507</v>
       </c>
       <c r="E8" s="1">
-        <f>C8/B8</f>
+        <f t="shared" si="0"/>
         <v>0.27244252644976535</v>
       </c>
     </row>
@@ -3969,7 +3970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E7898C6-66EA-45D8-84A9-54EDF6EE5E95}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -4007,7 +4008,7 @@
         <v>153392</v>
       </c>
       <c r="E2" s="1">
-        <f>C2/B2</f>
+        <f t="shared" ref="E2:E8" si="0">C2/B2</f>
         <v>0.29369077329698767</v>
       </c>
     </row>
@@ -4025,7 +4026,7 @@
         <v>199845</v>
       </c>
       <c r="E3" s="1">
-        <f>C3/B3</f>
+        <f t="shared" si="0"/>
         <v>0.27911565460172716</v>
       </c>
     </row>
@@ -4043,7 +4044,7 @@
         <v>171876</v>
       </c>
       <c r="E4" s="1">
-        <f>C4/B4</f>
+        <f t="shared" si="0"/>
         <v>0.29242346896767502</v>
       </c>
     </row>
@@ -4061,7 +4062,7 @@
         <v>126953</v>
       </c>
       <c r="E5" s="1">
-        <f>C5/B5</f>
+        <f t="shared" si="0"/>
         <v>0.28841993161818286</v>
       </c>
     </row>
@@ -4079,7 +4080,7 @@
         <v>98906</v>
       </c>
       <c r="E6" s="1">
-        <f>C6/B6</f>
+        <f t="shared" si="0"/>
         <v>0.29340239328451512</v>
       </c>
     </row>
@@ -4097,7 +4098,7 @@
         <v>69608</v>
       </c>
       <c r="E7" s="1">
-        <f>C7/B7</f>
+        <f t="shared" si="0"/>
         <v>0.30183948165533292</v>
       </c>
     </row>
@@ -4115,7 +4116,7 @@
         <v>204146</v>
       </c>
       <c r="E8" s="1">
-        <f>C8/B8</f>
+        <f t="shared" si="0"/>
         <v>0.33891614449247909</v>
       </c>
     </row>
@@ -4125,4 +4126,168 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51CC06E8-4D96-446E-81FF-3863C9FDB048}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>44238</v>
+      </c>
+      <c r="D2">
+        <v>12810</v>
+      </c>
+      <c r="E2">
+        <v>31428</v>
+      </c>
+      <c r="F2" s="1">
+        <f>D2/C2</f>
+        <v>0.28957005289570054</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>125084</v>
+      </c>
+      <c r="D3">
+        <v>38341</v>
+      </c>
+      <c r="E3">
+        <v>86743</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" ref="F3:F7" si="0">D3/C3</f>
+        <v>0.30652201720443861</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>96043</v>
+      </c>
+      <c r="D4">
+        <v>27301</v>
+      </c>
+      <c r="E4">
+        <v>68742</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="0"/>
+        <v>0.28425809272929836</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>43114</v>
+      </c>
+      <c r="D5">
+        <v>14068</v>
+      </c>
+      <c r="E5">
+        <v>29046</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.32629772231757664</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>13871</v>
+      </c>
+      <c r="D6">
+        <v>4953</v>
+      </c>
+      <c r="E6">
+        <v>8918</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.3570759137769447</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>5013</v>
+      </c>
+      <c r="D7">
+        <v>2074</v>
+      </c>
+      <c r="E7">
+        <v>2939</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.41372431677638138</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>